<commit_message>
Con cambios y errores
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drattek/W/REFACE/Import products/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2c706bb5fafd5b3c/Documentos/Importar Productos Odoo/odoo_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24483DD2-5A3E-1F4A-91FC-F0F2CCD7C3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{24483DD2-5A3E-1F4A-91FC-F0F2CCD7C3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{953E2264-A441-43E4-88CF-A66EA300E70D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{E6E0099B-C55A-F54D-82B9-E1B6267B876E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6E0099B-C55A-F54D-82B9-E1B6267B876E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
     <t>id_external</t>
   </si>
@@ -176,16 +176,16 @@
     <t>F00E164931-PESF00E164931-PES</t>
   </si>
   <si>
-    <t>DANY</t>
-  </si>
-  <si>
-    <t>IRVING</t>
-  </si>
-  <si>
-    <t>CHIDO</t>
-  </si>
-  <si>
-    <t>ONE</t>
+    <t>Oscar8</t>
+  </si>
+  <si>
+    <t>Irving8</t>
+  </si>
+  <si>
+    <t>Chido8</t>
+  </si>
+  <si>
+    <t>OCHO</t>
   </si>
 </sst>
 </file>
@@ -241,7 +241,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -560,12 +560,12 @@
   <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -648,13 +648,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>D2</f>
         <v>57190-PES</v>
       </c>
-      <c r="B2" t="s">
-        <v>46</v>
+      <c r="B2" t="str">
+        <f>_xlfn.CONCAT("desc",C2)</f>
+        <v>descOscar8</v>
       </c>
       <c r="C2" t="s">
         <v>46</v>
@@ -674,6 +675,10 @@
       <c r="H2" t="s">
         <v>29</v>
       </c>
+      <c r="I2" t="str">
+        <f>_xlfn.CONCAT(A2,B2,C2)</f>
+        <v>57190-PESdescOscar8Oscar8</v>
+      </c>
       <c r="J2" t="s">
         <v>30</v>
       </c>
@@ -717,13 +722,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A5" si="0">D3</f>
         <v>0986MF4395.-PES</v>
       </c>
-      <c r="B3" t="s">
-        <v>47</v>
+      <c r="B3" t="str">
+        <f>_xlfn.CONCAT("desc",C3)</f>
+        <v>descIrving8</v>
       </c>
       <c r="C3" t="s">
         <v>47</v>
@@ -743,6 +749,10 @@
       <c r="H3" t="s">
         <v>29</v>
       </c>
+      <c r="I3" t="str">
+        <f>_xlfn.CONCAT(A3,B3,C3)</f>
+        <v>0986MF4395.-PESdescIrving8Irving8</v>
+      </c>
       <c r="J3" t="s">
         <v>30</v>
       </c>
@@ -786,13 +796,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>9450905200-PES</v>
       </c>
-      <c r="B4" t="s">
-        <v>48</v>
+      <c r="B4" t="str">
+        <f>_xlfn.CONCAT("desc",C4)</f>
+        <v>descChido8</v>
       </c>
       <c r="C4" t="s">
         <v>48</v>
@@ -812,6 +823,10 @@
       <c r="H4" t="s">
         <v>29</v>
       </c>
+      <c r="I4" t="str">
+        <f>_xlfn.CONCAT(A4,B4,C4)</f>
+        <v>9450905200-PESdescChido8Chido8</v>
+      </c>
       <c r="J4" t="s">
         <v>30</v>
       </c>
@@ -855,13 +870,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>F00E164931-PES</v>
       </c>
-      <c r="B5" t="s">
-        <v>49</v>
+      <c r="B5" t="str">
+        <f>_xlfn.CONCAT("desc",C5)</f>
+        <v>descOCHO</v>
       </c>
       <c r="C5" t="s">
         <v>49</v>
@@ -880,6 +896,10 @@
       </c>
       <c r="H5" t="s">
         <v>29</v>
+      </c>
+      <c r="I5" t="str">
+        <f>_xlfn.CONCAT(A5,B5,C5)</f>
+        <v>F00E164931-PESdescOCHOOCHO</v>
       </c>
       <c r="J5" t="s">
         <v>30</v>
@@ -926,5 +946,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>